<commit_message>
Solved 27. Remove Element
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEEE21C-0859-4104-8E77-E68AC587E8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77873F0-51F2-4AA4-9236-3451086A2247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Category</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>two pointers, iterate from end;</t>
+  </si>
+  <si>
+    <t>Remove Element</t>
+  </si>
+  <si>
+    <t>two pointers, invisible elements;</t>
   </si>
 </sst>
 </file>
@@ -383,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -418,6 +424,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solved 125. Valid Palindrome
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77873F0-51F2-4AA4-9236-3451086A2247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F4C1C9-E568-4ECF-9606-B43AEAFB118E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Category</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>two pointers, invisible elements;</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>Valid Palindrome</t>
+  </si>
+  <si>
+    <t>two pointers, string;</t>
   </si>
 </sst>
 </file>
@@ -389,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,6 +444,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solved 912. Sort an Array
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F4C1C9-E568-4ECF-9606-B43AEAFB118E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4489C53E-B270-42D1-B02A-5D97902DA178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Category</t>
   </si>
@@ -58,13 +58,22 @@
   </si>
   <si>
     <t>two pointers, string;</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>Sort an Array</t>
+  </si>
+  <si>
+    <t>merge sort, d&amp;c, recursion;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,8 +96,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,6 +114,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -114,10 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,6 +478,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solved 108. Convert Sorted Array to Binary Search Tree
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4489C53E-B270-42D1-B02A-5D97902DA178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9569A319-866B-48CE-B4BC-4DB0A17A3E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Category</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t>merge sort, d&amp;c, recursion;</t>
+  </si>
+  <si>
+    <t>D&amp;C</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>d&amp;c, recursion;</t>
   </si>
 </sst>
 </file>
@@ -421,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,6 +498,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solved 215. Kth Largest Element in an Array
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9569A319-866B-48CE-B4BC-4DB0A17A3E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02C24C-0CC0-4C06-92E2-C59171778754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Category</t>
   </si>
@@ -69,13 +69,22 @@
     <t>merge sort, d&amp;c, recursion;</t>
   </si>
   <si>
-    <t>D&amp;C</t>
-  </si>
-  <si>
     <t>Convert Sorted Array to Binary Search Tree</t>
   </si>
   <si>
     <t>d&amp;c, recursion;</t>
+  </si>
+  <si>
+    <t>Heap</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>priority queue;</t>
+  </si>
+  <si>
+    <t>Divide &amp; Conquer</t>
   </si>
 </sst>
 </file>
@@ -430,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,13 +509,24 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solved 35. Search Insert Position
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E02C24C-0CC0-4C06-92E2-C59171778754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFE6BAC-B41D-4345-B619-75FDD0C6CA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Category</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Divide &amp; Conquer</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>discrete binary search, lower_bound;</t>
   </si>
 </sst>
 </file>
@@ -439,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,6 +538,17 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solved 34. Find First and Last Position of Element in Sorted Array
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFE6BAC-B41D-4345-B619-75FDD0C6CA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8EE537-859A-49B7-9BB2-625DB0653E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Category</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>discrete binary search, lower_bound;</t>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+  </si>
+  <si>
+    <t>discrete binary search, l&amp;r, equal_range;</t>
   </si>
 </sst>
 </file>
@@ -448,16 +454,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+    <col min="2" max="2" width="47.33203125" customWidth="1"/>
     <col min="3" max="3" width="130.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -549,6 +555,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solved 74. Search a 2D Matrix
</commit_message>
<xml_diff>
--- a/cheat sheet.xlsx
+++ b/cheat sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\alg\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8EE537-859A-49B7-9BB2-625DB0653E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7532EB68-F0BB-4C1B-9640-F832374B87ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8508" yWindow="1836" windowWidth="14340" windowHeight="8856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Category</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>discrete binary search, l&amp;r, equal_range;</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>discrete binary search, 2D arrays;</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -566,6 +572,17 @@
         <v>24</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>